<commit_message>
Corrección de errores en control de documentacion, optimización del código
</commit_message>
<xml_diff>
--- a/-110001.xlsx
+++ b/-110001.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="70">
   <si>
     <t xml:space="preserve">           CONDICIONES DE TRABAJO, INSPECCION Y COMENTARIOS PARA PIEZAS LIBERADAS</t>
   </si>
@@ -150,6 +150,12 @@
     <t>19/09/2024</t>
   </si>
   <si>
+    <t>25/09/2024</t>
+  </si>
+  <si>
+    <t>26/09/2024</t>
+  </si>
+  <si>
     <t>110001</t>
   </si>
   <si>
@@ -215,24 +221,33 @@
     <t>4</t>
   </si>
   <si>
+    <t>RAYAS/REBABAS DIAM. EXTERIOR
+NO PERMITIDAS</t>
+  </si>
+  <si>
     <t>RAYAS/REBABAS INCOMPLETA
 NO PERMITIDAS</t>
   </si>
   <si>
-    <t>RAYAS/REBABAS DIAM. EXTERIOR
-NO PERMITIDAS</t>
+    <t>NEGATIVO</t>
+  </si>
+  <si>
+    <t>SI</t>
   </si>
   <si>
     <t>1.381</t>
   </si>
   <si>
-    <t>SI</t>
+    <t>po09</t>
   </si>
   <si>
-    <t>NEGATIVO</t>
+    <t>951623</t>
   </si>
   <si>
-    <t>po09</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>102164</t>
   </si>
 </sst>
 </file>
@@ -242,7 +257,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="49">
+  <fonts count="65">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -336,6 +351,70 @@
     <font>
       <name val="Calibri"/>
       <sz val="7.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="6.0"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1119,7 +1198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1"/>
@@ -1563,6 +1642,60 @@
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="57" xfId="0" applyFont="true" applyBorder="true">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2585,20 +2718,28 @@
       <c r="C9" s="29">
         <v>3</v>
       </c>
-      <c r="D9" s="50"/>
+      <c r="D9" s="50" t="s">
+        <v>38</v>
+      </c>
       <c r="E9" s="51"/>
       <c r="F9" s="51"/>
       <c r="G9" s="51"/>
       <c r="H9" s="26"/>
-      <c r="I9" s="51"/>
+      <c r="I9" s="51" t="s">
+        <v>34</v>
+      </c>
       <c r="J9" s="51"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="51"/>
+      <c r="L9" s="51" t="s">
+        <v>35</v>
+      </c>
       <c r="M9" s="51"/>
       <c r="N9" s="51"/>
       <c r="O9" s="51"/>
       <c r="P9" s="26"/>
-      <c r="Q9" s="51"/>
+      <c r="Q9" s="51" t="s">
+        <v>36</v>
+      </c>
       <c r="R9" s="51"/>
       <c r="S9" s="51"/>
       <c r="T9" s="51"/>
@@ -2631,20 +2772,28 @@
       <c r="C10" s="29">
         <v>4</v>
       </c>
-      <c r="D10" s="50"/>
+      <c r="D10" s="50" t="s">
+        <v>39</v>
+      </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
       <c r="H10" s="26"/>
-      <c r="I10" s="51"/>
+      <c r="I10" s="51" t="s">
+        <v>34</v>
+      </c>
       <c r="J10" s="51"/>
       <c r="K10" s="26"/>
-      <c r="L10" s="51"/>
+      <c r="L10" s="51" t="s">
+        <v>35</v>
+      </c>
       <c r="M10" s="51"/>
       <c r="N10" s="51"/>
       <c r="O10" s="51"/>
       <c r="P10" s="26"/>
-      <c r="Q10" s="51"/>
+      <c r="Q10" s="51" t="s">
+        <v>36</v>
+      </c>
       <c r="R10" s="51"/>
       <c r="S10" s="51"/>
       <c r="T10" s="51"/>
@@ -6050,7 +6199,7 @@
       <c r="L3" s="97"/>
       <c r="M3" s="97"/>
       <c r="N3" s="98" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O3" s="98"/>
       <c r="P3" s="98"/>
@@ -6061,7 +6210,7 @@
       <c r="S3" s="100"/>
       <c r="T3" s="100"/>
       <c r="U3" s="98" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="V3" s="98"/>
       <c r="W3" s="98"/>
@@ -6071,7 +6220,7 @@
       <c r="Y3" s="100"/>
       <c r="Z3" s="100"/>
       <c r="AA3" s="98" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="AB3" s="98"/>
       <c r="AC3" s="98"/>
@@ -6129,7 +6278,7 @@
         <v>18</v>
       </c>
       <c r="M5" s="113" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N5" s="114"/>
       <c r="O5" s="5"/>
@@ -6137,7 +6286,7 @@
         <v>19</v>
       </c>
       <c r="Q5" s="115" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="R5" s="115"/>
       <c r="S5" s="2"/>
@@ -6172,11 +6321,11 @@
       <c r="H6" s="71"/>
       <c r="I6" s="75"/>
       <c r="J6" s="127" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K6" s="80"/>
       <c r="L6" s="127" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M6" s="80"/>
       <c r="N6" s="127"/>
@@ -6311,35 +6460,35 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="136" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B10" s="137" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="138" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D10" s="139" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E10" s="140" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F10" s="141" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G10" s="142" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H10" s="143" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I10" s="135" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J10" s="135"/>
       <c r="K10" s="135" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="L10" s="135"/>
       <c r="M10" s="126"/>
@@ -6363,35 +6512,35 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="145" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B11" s="146" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="147" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11" s="148" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E11" s="149" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F11" s="150" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G11" s="151" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H11" s="152" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I11" s="144" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J11" s="144"/>
       <c r="K11" s="144" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L11" s="144"/>
       <c r="M11" s="126"/>
@@ -7416,7 +7565,7 @@
       <c r="L41" s="97"/>
       <c r="M41" s="97"/>
       <c r="N41" s="98" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O41" s="98"/>
       <c r="P41" s="98"/>
@@ -7427,7 +7576,7 @@
       <c r="S41" s="100"/>
       <c r="T41" s="100"/>
       <c r="U41" s="98" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="V41" s="98"/>
       <c r="W41" s="98"/>
@@ -7437,7 +7586,7 @@
       <c r="Y41" s="100"/>
       <c r="Z41" s="100"/>
       <c r="AA41" s="98" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AB41" s="98"/>
       <c r="AC41" s="98"/>
@@ -7505,7 +7654,7 @@
         <v>20</v>
       </c>
       <c r="U43" s="115" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="V43" s="115"/>
       <c r="W43" s="2"/>
@@ -7534,7 +7683,7 @@
       <c r="H44" s="71"/>
       <c r="I44" s="75"/>
       <c r="J44" s="77" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K44" s="80"/>
       <c r="L44" s="77"/>
@@ -7671,31 +7820,31 @@
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="154" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B48" s="155" t="s">
         <v>33</v>
       </c>
       <c r="C48" s="156" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D48" s="157" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E48" s="158" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F48" s="159" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G48" s="160" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H48" s="161" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I48" s="153" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J48" s="153"/>
       <c r="K48" s="101"/>
@@ -8756,7 +8905,7 @@
       <c r="L79" s="97"/>
       <c r="M79" s="97"/>
       <c r="N79" s="98" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O79" s="98"/>
       <c r="P79" s="98"/>
@@ -8767,7 +8916,7 @@
       <c r="S79" s="100"/>
       <c r="T79" s="100"/>
       <c r="U79" s="98" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="V79" s="98"/>
       <c r="W79" s="98"/>
@@ -8777,7 +8926,7 @@
       <c r="Y79" s="100"/>
       <c r="Z79" s="100"/>
       <c r="AA79" s="98" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AB79" s="98"/>
       <c r="AC79" s="98"/>
@@ -8850,7 +8999,9 @@
       <c r="X81" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="Y81" s="115"/>
+      <c r="Y81" s="115" t="s">
+        <v>45</v>
+      </c>
       <c r="Z81" s="115"/>
       <c r="AA81" s="2"/>
       <c r="AB81" s="11" t="s">
@@ -8872,19 +9023,19 @@
       <c r="H82" s="71"/>
       <c r="I82" s="75"/>
       <c r="J82" s="77" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="K82" s="80"/>
       <c r="L82" s="77" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="M82" s="80"/>
       <c r="N82" s="77" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="O82" s="87"/>
       <c r="P82" s="77" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="Q82" s="87"/>
       <c r="R82" s="77"/>
@@ -9015,43 +9166,43 @@
     </row>
     <row r="86" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="163" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B86" s="164" t="s">
         <v>37</v>
       </c>
       <c r="C86" s="165" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D86" s="166" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E86" s="167" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F86" s="168" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G86" s="169" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H86" s="170" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I86" s="162" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J86" s="162"/>
       <c r="K86" s="162" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="L86" s="162"/>
       <c r="M86" s="162" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="N86" s="162"/>
       <c r="O86" s="162" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="P86" s="162"/>
       <c r="Q86" s="101"/>
@@ -9070,24 +9221,46 @@
       <c r="AD86" s="101"/>
     </row>
     <row r="87" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="45">
-        <v>2</v>
-      </c>
-      <c r="B87" s="36"/>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="37"/>
-      <c r="G87" s="37"/>
-      <c r="H87" s="37"/>
-      <c r="I87" s="101"/>
-      <c r="J87" s="101"/>
-      <c r="K87" s="101"/>
-      <c r="L87" s="101"/>
-      <c r="M87" s="101"/>
-      <c r="N87" s="101"/>
-      <c r="O87" s="101"/>
-      <c r="P87" s="101"/>
+      <c r="A87" s="172" t="s">
+        <v>60</v>
+      </c>
+      <c r="B87" s="173" t="s">
+        <v>38</v>
+      </c>
+      <c r="C87" s="174" t="s">
+        <v>67</v>
+      </c>
+      <c r="D87" s="175" t="s">
+        <v>53</v>
+      </c>
+      <c r="E87" s="176" t="s">
+        <v>54</v>
+      </c>
+      <c r="F87" s="177" t="s">
+        <v>55</v>
+      </c>
+      <c r="G87" s="178" t="s">
+        <v>46</v>
+      </c>
+      <c r="H87" s="179" t="s">
+        <v>56</v>
+      </c>
+      <c r="I87" s="171" t="s">
+        <v>58</v>
+      </c>
+      <c r="J87" s="171"/>
+      <c r="K87" s="171" t="s">
+        <v>58</v>
+      </c>
+      <c r="L87" s="171"/>
+      <c r="M87" s="171" t="s">
+        <v>58</v>
+      </c>
+      <c r="N87" s="171"/>
+      <c r="O87" s="171" t="s">
+        <v>65</v>
+      </c>
+      <c r="P87" s="171"/>
       <c r="Q87" s="101"/>
       <c r="R87" s="101"/>
       <c r="S87" s="101"/>
@@ -10074,7 +10247,7 @@
       <c r="L117" s="97"/>
       <c r="M117" s="97"/>
       <c r="N117" s="98" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O117" s="98"/>
       <c r="P117" s="98"/>
@@ -10085,7 +10258,7 @@
       <c r="S117" s="100"/>
       <c r="T117" s="100"/>
       <c r="U117" s="98" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="V117" s="98"/>
       <c r="W117" s="98"/>
@@ -10094,7 +10267,9 @@
       </c>
       <c r="Y117" s="100"/>
       <c r="Z117" s="100"/>
-      <c r="AA117" s="98"/>
+      <c r="AA117" s="98" t="s">
+        <v>44</v>
+      </c>
       <c r="AB117" s="98"/>
       <c r="AC117" s="98"/>
       <c r="AD117" s="98"/>
@@ -10173,7 +10348,7 @@
         <v>22</v>
       </c>
       <c r="AC119" s="115" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AD119" s="115"/>
     </row>
@@ -10189,7 +10364,9 @@
       <c r="G120" s="70"/>
       <c r="H120" s="71"/>
       <c r="I120" s="75"/>
-      <c r="J120" s="77"/>
+      <c r="J120" s="77" t="s">
+        <v>47</v>
+      </c>
       <c r="K120" s="80"/>
       <c r="L120" s="77"/>
       <c r="M120" s="80"/>
@@ -10324,18 +10501,34 @@
       <c r="AD123" s="79"/>
     </row>
     <row r="124" spans="1:30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="45">
-        <v>1</v>
-      </c>
-      <c r="B124" s="36"/>
-      <c r="C124" s="38"/>
-      <c r="D124" s="38"/>
-      <c r="E124" s="37"/>
-      <c r="F124" s="37"/>
-      <c r="G124" s="37"/>
-      <c r="H124" s="37"/>
-      <c r="I124" s="101"/>
-      <c r="J124" s="101"/>
+      <c r="A124" s="181" t="s">
+        <v>68</v>
+      </c>
+      <c r="B124" s="182" t="s">
+        <v>39</v>
+      </c>
+      <c r="C124" s="183" t="s">
+        <v>69</v>
+      </c>
+      <c r="D124" s="184" t="s">
+        <v>53</v>
+      </c>
+      <c r="E124" s="185" t="s">
+        <v>54</v>
+      </c>
+      <c r="F124" s="186" t="s">
+        <v>55</v>
+      </c>
+      <c r="G124" s="187" t="s">
+        <v>46</v>
+      </c>
+      <c r="H124" s="188" t="s">
+        <v>56</v>
+      </c>
+      <c r="I124" s="180" t="s">
+        <v>49</v>
+      </c>
+      <c r="J124" s="180"/>
       <c r="K124" s="101"/>
       <c r="L124" s="101"/>
       <c r="M124" s="101"/>

</xml_diff>